<commit_message>
Fixed rule that sometimes affected convergence
</commit_message>
<xml_diff>
--- a/areas.xlsx
+++ b/areas.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brene\Dropbox\shift_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0BD11CEA-BE2F-444D-A568-706151D80DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D3CECA-6BD7-430C-8FEF-F1F43AE1D22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="areas" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,12 +635,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -995,11 +994,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="A2:H33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1015,28 +1014,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1062,7 +1061,6 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1086,7 +1084,6 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1110,7 +1107,6 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1134,7 +1130,6 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1158,7 +1153,6 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1182,7 +1176,6 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1206,7 +1199,6 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1230,7 +1222,6 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1254,7 +1245,6 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1278,7 +1268,6 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -1302,7 +1291,6 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1326,7 +1314,6 @@
       <c r="G13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -1350,7 +1337,6 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -1371,8 +1357,9 @@
       <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -1396,9 +1383,8 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1420,9 +1406,8 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1444,9 +1429,8 @@
       <c r="G18" s="1">
         <v>1</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1468,9 +1452,8 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1492,137 +1475,6 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>